<commit_message>
Article details page request finished
</commit_message>
<xml_diff>
--- a/dummy_database.xlsx
+++ b/dummy_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denysil/Documents/NOTES/CDM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD1E9B3-776C-CF46-800E-E9797C8F7B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16FCC02-8ECA-5844-9AB2-88304BE6E4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,13 +156,13 @@
     <t>tags</t>
   </si>
   <si>
-    <t>list, of, nsmi, tags</t>
-  </si>
-  <si>
-    <t>of, nsmi, tags</t>
-  </si>
-  <si>
     <t>list, tags</t>
+  </si>
+  <si>
+    <t>1.1.list, 2.2of, 3.3.nsmi, tags</t>
+  </si>
+  <si>
+    <t>1.3.of, 2.3.nsmi, tags</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -603,7 +603,7 @@
         <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
@@ -632,7 +632,7 @@
         <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
         <v>34</v>
@@ -661,7 +661,7 @@
         <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
         <v>39</v>

</xml_diff>